<commit_message>
smartvac-fhir xlsx mapping updated
</commit_message>
<xml_diff>
--- a/examples/smartvac/smart-vacc-cert-fhir-mapping.xlsx
+++ b/examples/smartvac/smart-vacc-cert-fhir-mapping.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
-    <t xml:space="preserve">WHO SmartVacc Parameter</t>
+    <t xml:space="preserve">SmartVacc Parameter</t>
   </si>
   <si>
     <t xml:space="preserve">Type</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">resource.resourceType[“Location”].name</t>
   </si>
   <si>
-    <t xml:space="preserve">id also present in source – better?</t>
+    <t xml:space="preserve">id also present in source – id better?</t>
   </si>
 </sst>
 </file>
@@ -133,6 +133,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,6 +155,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -161,6 +163,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -335,16 +338,16 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.31"/>
   </cols>
   <sheetData>

</xml_diff>